<commit_message>
Fixed formulas Added RDP accessibility
</commit_message>
<xml_diff>
--- a/VESS.xlsx
+++ b/VESS.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/USB/Users/timb/Security/Research/Personal/Vulnerability Analysis/vulnerability-analysis-trunk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B90A8EFE-8F0A-2D49-8B37-9FCE06E86823}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CDC036-9CDC-2C40-A54E-B729CBB6B04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="26740" windowHeight="13540" activeTab="1" xr2:uid="{06B14344-FF18-BC43-ABAB-FDE9C1AD93D4}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13280" activeTab="1" xr2:uid="{06B14344-FF18-BC43-ABAB-FDE9C1AD93D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="2" r:id="rId1"/>
     <sheet name="Examples" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="74">
   <si>
     <t>Authentication required</t>
   </si>
@@ -254,6 +256,9 @@
   </si>
   <si>
     <t>CVE-2020-17530</t>
+  </si>
+  <si>
+    <t>RDP accessible</t>
   </si>
 </sst>
 </file>
@@ -611,7 +616,7 @@
   <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1177,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE64958-2A1A-0440-B9EF-576B082BD9B7}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1293,67 +1298,67 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B3">
-        <f>SUMIF(Matrix!A3:A9, B2, Matrix!B3:B9)</f>
+        <f>SUMIF(Matrix!$A$3:$A$6, B2, Matrix!$B$3:$B$6)</f>
         <v>0.2</v>
       </c>
       <c r="C3">
-        <f>SUMIF(Matrix!C3:C8, C2, Matrix!D3:D8)</f>
+        <f>SUMIF(Matrix!$C$3:$C$8, C2, Matrix!$D$3:$D$8)</f>
         <v>0.05</v>
       </c>
       <c r="D3">
-        <f>SUMIF(Matrix!E3:E8, D2, Matrix!F3:F8)</f>
+        <f>SUMIF(Matrix!$E$3:$E$8, D2, Matrix!$F$3:$F$8)</f>
         <v>0.1</v>
       </c>
       <c r="E3">
-        <f>SUMIF(Matrix!G3:G8, E2, Matrix!H3:H8)</f>
+        <f>SUMIF(Matrix!$G$7:$G$8, E2, Matrix!$H$3:$H$7)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>SUMIF(Matrix!$I$3:$I$6, F2, Matrix!$J$3:$J$6)</f>
         <v>0.05</v>
       </c>
-      <c r="F3">
-        <f>SUMIF(Matrix!I3:I8, F2, Matrix!J3:J8)</f>
+      <c r="G3">
+        <f>SUMIF(Matrix!$K$3:$K$6, G2, Matrix!$L$3:$L$6)</f>
         <v>0.05</v>
       </c>
-      <c r="G3">
-        <f>SUMIF(Matrix!K3:K8, G2, Matrix!L3:L8)</f>
+      <c r="H3">
+        <f>SUMIF(Matrix!$M$3:$M$9, H2, Matrix!$N$3:$N$9)</f>
         <v>0.05</v>
       </c>
-      <c r="H3">
-        <f>SUMIF(Matrix!M3:M9, H2, Matrix!N3:N9)</f>
-        <v>0.05</v>
-      </c>
       <c r="I3">
-        <f>SUMIF(Matrix!O3:O9, I2, Matrix!P3:P9)</f>
+        <f>SUMIF(Matrix!$O$3:$O$6, I2, Matrix!$P$3:$P$6)</f>
         <v>0.1</v>
       </c>
       <c r="J3">
-        <f>SUMIF(Matrix!Q3:Q9, J2, Matrix!R3:R9)</f>
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J2, Matrix!$R$3:$R$8)</f>
         <v>0.1</v>
       </c>
       <c r="K3">
-        <f>SUMIF(Matrix!S3:S9, K2, Matrix!T3:T9)</f>
+        <f>SUMIF(Matrix!$S$3:$S$6, K2, Matrix!$T$3:$T$6)</f>
         <v>0</v>
       </c>
       <c r="L3">
-        <f ca="1">SUMIF(Matrix!U3:V9, L2, Matrix!V3:V9)</f>
+        <f>SUMIF(Matrix!$U$3:$U$6, L2, Matrix!$V$3:$V$6)</f>
         <v>0.3</v>
       </c>
       <c r="M3">
-        <f>SUMIF(Matrix!W3:W9, M2, Matrix!X3:X9)</f>
+        <f>SUMIF(Matrix!$W$3:$W$6, M2, Matrix!$X$3:$X$6)</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f>SUMIF(Matrix!Y3:Y7, N2, Matrix!Z3:Z7)</f>
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N2, Matrix!$Z$3:$Z$7)</f>
         <v>0.1</v>
       </c>
       <c r="O3">
-        <f>SUMIF(Matrix!AA3:AA7, O2, Matrix!AB3:AB7)</f>
+        <f>SUMIF(Matrix!$AA$3:$AA$7, O2, Matrix!$AB$3:$AB$7)</f>
         <v>0.1</v>
       </c>
       <c r="P3">
         <f>SUM(B3:G3)</f>
-        <v>0.49999999999999994</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="Q3">
-        <f ca="1">SUM(H3:M3)</f>
+        <f>SUM(H3:M3)</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="R3">
@@ -1361,7 +1366,7 @@
         <v>0.2</v>
       </c>
       <c r="S3" t="b">
-        <f ca="1">OR(IF(P3&gt;1.9, TRUE), IF(Q3&gt;1.5, TRUE), AND(IF(P3&gt;1.2, TRUE), IF(Q3&gt;1.2, TRUE)))</f>
+        <f>OR(IF(P3&gt;1.9, TRUE), IF(Q3&gt;1.5, TRUE), AND(IF(P3&gt;1.2, TRUE), IF(Q3&gt;1.2, TRUE)))</f>
         <v>0</v>
       </c>
     </row>
@@ -1414,55 +1419,55 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B5">
-        <f>SUMIF(Matrix!A3:A9, B4, Matrix!B3:B9)</f>
+        <f>SUMIF(Matrix!$A$3:$A$6, B4, Matrix!$B$3:$B$6)</f>
         <v>0.4</v>
       </c>
       <c r="C5">
-        <f>SUMIF(Matrix!C3:C9, C4, Matrix!D3:D9)</f>
+        <f>SUMIF(Matrix!$C$3:$C$8, C4, Matrix!$D$3:$D$8)</f>
         <v>0.4</v>
       </c>
       <c r="D5">
-        <f>SUMIF(Matrix!E3:E9, D4, Matrix!F3:F9)</f>
+        <f>SUMIF(Matrix!$E$3:$E$8, D4, Matrix!$F$3:$F$8)</f>
         <v>0.4</v>
       </c>
       <c r="E5">
-        <f>SUMIF(Matrix!G3:G9, E4, Matrix!H3:H9)</f>
-        <v>0.3</v>
+        <f>SUMIF(Matrix!$G$7:$G$8, E4, Matrix!$H$3:$H$7)</f>
+        <v>0</v>
       </c>
       <c r="F5">
-        <f>SUMIF(Matrix!I3:I9, F4, Matrix!J3:J9)</f>
+        <f>SUMIF(Matrix!$I$3:$I$6, F4, Matrix!$J$3:$J$6)</f>
         <v>0.4</v>
       </c>
       <c r="G5">
-        <f>SUMIF(Matrix!K3:K9, G4, Matrix!L3:L9)</f>
+        <f>SUMIF(Matrix!$K$3:$K$6, G4, Matrix!$L$3:$L$6)</f>
         <v>0.4</v>
       </c>
       <c r="H5">
-        <f>SUMIF(Matrix!M3:M9, H4, Matrix!N3:N9)</f>
+        <f>SUMIF(Matrix!$M$3:$M$9, H4, Matrix!$N$3:$N$9)</f>
         <v>0.1</v>
       </c>
       <c r="I5">
-        <f>SUMIF(Matrix!O3:O9, I4, Matrix!P3:P9)</f>
+        <f>SUMIF(Matrix!$O$3:$O$6, I4, Matrix!$P$3:$P$6)</f>
         <v>0.1</v>
       </c>
       <c r="J5">
-        <f>SUMIF(Matrix!Q3:Q9, J4, Matrix!R3:R9)</f>
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J4, Matrix!$R$3:$R$8)</f>
         <v>0.05</v>
       </c>
       <c r="K5">
-        <f>SUMIF(Matrix!S3:S9, K4, Matrix!T3:T9)</f>
+        <f>SUMIF(Matrix!$S$3:$S$6, K4, Matrix!$T$3:$T$6)</f>
         <v>0.2</v>
       </c>
       <c r="L5">
-        <f>SUMIF(Matrix!U3:U9, L4, Matrix!V3:V9)</f>
+        <f>SUMIF(Matrix!$U$3:$U$6, L4, Matrix!$V$3:$V$6)</f>
         <v>0</v>
       </c>
       <c r="M5">
-        <f>SUMIF(Matrix!W3:W9, M4, Matrix!X3:X9)</f>
+        <f>SUMIF(Matrix!$W$3:$W$6, M4, Matrix!$X$3:$X$6)</f>
         <v>0</v>
       </c>
       <c r="N5">
-        <f>SUMIF(Matrix!Y3:Y7, N4, Matrix!Z3:Z7)</f>
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N4, Matrix!$Z$3:$Z$7)</f>
         <v>0.1</v>
       </c>
       <c r="O5">
@@ -1471,7 +1476,7 @@
       </c>
       <c r="P5">
         <f>SUM(B5:G5)</f>
-        <v>2.3000000000000003</v>
+        <v>2</v>
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5:Q19" si="0">SUM(H5:M5)</f>
@@ -1535,55 +1540,55 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B7">
-        <f>SUMIF(Matrix!A3:A9, B6, Matrix!B3:B9)</f>
+        <f>SUMIF(Matrix!$A$3:$A$6, B6, Matrix!$B$3:$B$6)</f>
         <v>0.3</v>
       </c>
       <c r="C7">
-        <f>SUMIF(Matrix!C3:C8, C6, Matrix!D3:D8)</f>
+        <f>SUMIF(Matrix!$C$3:$C$8, C6, Matrix!$D$3:$D$8)</f>
         <v>0.4</v>
       </c>
       <c r="D7">
-        <f>SUMIF(Matrix!E3:E8, D6, Matrix!F3:F8)</f>
+        <f>SUMIF(Matrix!$E$3:$E$8, D6, Matrix!$F$3:$F$8)</f>
         <v>0.4</v>
       </c>
       <c r="E7">
-        <f>SUMIF(Matrix!G3:G8, E6, Matrix!H3:H8)</f>
-        <v>0.23749999999999999</v>
+        <f>SUMIF(Matrix!$G$7:$G$8, E6, Matrix!$H$3:$H$7)</f>
+        <v>0.4</v>
       </c>
       <c r="F7">
-        <f>SUMIF(Matrix!I3:I8, F6, Matrix!J3:J8)</f>
+        <f>SUMIF(Matrix!$I$3:$I$6, F6, Matrix!$J$3:$J$6)</f>
         <v>0.05</v>
       </c>
       <c r="G7">
-        <f>SUMIF(Matrix!K3:K8, G6, Matrix!L3:L8)</f>
+        <f>SUMIF(Matrix!$K$3:$K$6, G6, Matrix!$L$3:$L$6)</f>
         <v>0.05</v>
       </c>
       <c r="H7">
-        <f>SUMIF(Matrix!M3:M9, H6, Matrix!N3:N9)</f>
+        <f>SUMIF(Matrix!$M$3:$M$9, H6, Matrix!$N$3:$N$9)</f>
         <v>0.17500000000000002</v>
       </c>
       <c r="I7">
-        <f>SUMIF(Matrix!O3:O9, I6, Matrix!P3:P9)</f>
+        <f>SUMIF(Matrix!$O$3:$O$6, I6, Matrix!$P$3:$P$6)</f>
         <v>0.1</v>
       </c>
       <c r="J7">
-        <f>SUMIF(Matrix!Q3:Q9, J6, Matrix!R3:R9)</f>
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J6, Matrix!$R$3:$R$8)</f>
         <v>0.25</v>
       </c>
       <c r="K7">
-        <f>SUMIF(Matrix!S3:S9, K6, Matrix!T3:T9)</f>
+        <f>SUMIF(Matrix!$S$3:$S$6, K6, Matrix!$T$3:$T$6)</f>
         <v>0.2</v>
       </c>
       <c r="L7">
-        <f ca="1">SUMIF(Matrix!U3:V9, L6, Matrix!V3:V9)</f>
+        <f>SUMIF(Matrix!$U$3:$U$6, L6, Matrix!$V$3:$V$6)</f>
         <v>0.3</v>
       </c>
       <c r="M7">
-        <f>SUMIF(Matrix!W3:W9, M6, Matrix!X3:X9)</f>
+        <f>SUMIF(Matrix!$W$3:$W$6, M6, Matrix!$X$3:$X$6)</f>
         <v>0</v>
       </c>
       <c r="N7">
-        <f>SUMIF(Matrix!Y3:Y7, N6, Matrix!Z3:Z7)</f>
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N6, Matrix!$Z$3:$Z$7)</f>
         <v>0.3</v>
       </c>
       <c r="O7">
@@ -1592,10 +1597,10 @@
       </c>
       <c r="P7">
         <f>SUM(B7:G7)</f>
-        <v>1.4375000000000002</v>
+        <v>1.6</v>
       </c>
       <c r="Q7">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>1.0250000000000001</v>
       </c>
       <c r="R7">
@@ -1603,7 +1608,7 @@
         <v>0.6</v>
       </c>
       <c r="S7" t="b">
-        <f ca="1">OR(IF(P7&gt;1.9, TRUE), IF(Q7&gt;1.5, TRUE), AND(IF(P7&gt;1.2, TRUE), IF(Q7&gt;1.2, TRUE)))</f>
+        <f>OR(IF(P7&gt;1.9, TRUE), IF(Q7&gt;1.5, TRUE), AND(IF(P7&gt;1.2, TRUE), IF(Q7&gt;1.2, TRUE)))</f>
         <v>0</v>
       </c>
     </row>
@@ -1656,55 +1661,55 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9">
-        <f>SUMIF(Matrix!A3:A9, B8, Matrix!B3:B9)</f>
+        <f>SUMIF(Matrix!$A$3:$A$6, B8, Matrix!$B$3:$B$6)</f>
         <v>0.3</v>
       </c>
       <c r="C9">
-        <f>SUMIF(Matrix!C3:C9, C8, Matrix!D3:D9)</f>
+        <f>SUMIF(Matrix!$C$3:$C$8, C8, Matrix!$D$3:$D$8)</f>
         <v>0.4</v>
       </c>
       <c r="D9">
-        <f>SUMIF(Matrix!E3:E9, D8, Matrix!F3:F9)</f>
+        <f>SUMIF(Matrix!$E$3:$E$8, D8, Matrix!$F$3:$F$8)</f>
         <v>0.1</v>
       </c>
       <c r="E9">
-        <f>SUMIF(Matrix!G3:G9, E8, Matrix!H3:H9)</f>
-        <v>0.3</v>
+        <f>SUMIF(Matrix!$G$7:$G$8, E8, Matrix!$H$3:$H$7)</f>
+        <v>0</v>
       </c>
       <c r="F9">
-        <f>SUMIF(Matrix!I3:I9, F8, Matrix!J3:J9)</f>
+        <f>SUMIF(Matrix!$I$3:$I$6, F8, Matrix!$J$3:$J$6)</f>
         <v>0.4</v>
       </c>
       <c r="G9">
-        <f>SUMIF(Matrix!K3:K9, G8, Matrix!L3:L9)</f>
+        <f>SUMIF(Matrix!$K$3:$K$6, G8, Matrix!$L$3:$L$6)</f>
         <v>0.4</v>
       </c>
       <c r="H9">
-        <f>SUMIF(Matrix!M3:M9, H8, Matrix!N3:N9)</f>
+        <f>SUMIF(Matrix!$M$3:$M$9, H8, Matrix!$N$3:$N$9)</f>
         <v>0.1</v>
       </c>
       <c r="I9">
-        <f>SUMIF(Matrix!O3:O9, I8, Matrix!P3:P9)</f>
+        <f>SUMIF(Matrix!$O$3:$O$6, I8, Matrix!$P$3:$P$6)</f>
         <v>0.2</v>
       </c>
       <c r="J9">
-        <f>SUMIF(Matrix!Q3:Q9, J8, Matrix!R3:R9)</f>
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J8, Matrix!$R$3:$R$8)</f>
         <v>0.25</v>
       </c>
       <c r="K9">
-        <f>SUMIF(Matrix!S3:S9, K8, Matrix!T3:T9)</f>
+        <f>SUMIF(Matrix!$S$3:$S$6, K8, Matrix!$T$3:$T$6)</f>
         <v>0.4</v>
       </c>
       <c r="L9">
-        <f>SUMIF(Matrix!U3:U9, L8, Matrix!V3:V9)</f>
+        <f>SUMIF(Matrix!$U$3:$U$6, L8, Matrix!$V$3:$V$6)</f>
         <v>0.4</v>
       </c>
       <c r="M9">
-        <f>SUMIF(Matrix!W3:W9, M8, Matrix!X3:X9)</f>
+        <f>SUMIF(Matrix!$W$3:$W$6, M8, Matrix!$X$3:$X$6)</f>
         <v>0.4</v>
       </c>
       <c r="N9">
-        <f>SUMIF(Matrix!Y3:Y7, N8, Matrix!Z3:Z7)</f>
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N8, Matrix!$Z$3:$Z$7)</f>
         <v>0.1</v>
       </c>
       <c r="O9">
@@ -1713,7 +1718,7 @@
       </c>
       <c r="P9">
         <f>SUM(B9:G9)</f>
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
@@ -1777,55 +1782,55 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B11">
-        <f>SUMIF(Matrix!A3:A9, B10, Matrix!B3:B9)</f>
+        <f>SUMIF(Matrix!$A$3:$A$6, B10, Matrix!$B$3:$B$6)</f>
         <v>0.3</v>
       </c>
       <c r="C11">
-        <f>SUMIF(Matrix!C3:C8, C10, Matrix!D3:D8)</f>
+        <f>SUMIF(Matrix!$C$3:$C$8, C10, Matrix!$D$3:$D$8)</f>
         <v>0.1</v>
       </c>
       <c r="D11">
-        <f>SUMIF(Matrix!E3:E8, D10, Matrix!F3:F8)</f>
+        <f>SUMIF(Matrix!$E$3:$E$8, D10, Matrix!$F$3:$F$8)</f>
         <v>0.4</v>
       </c>
       <c r="E11">
-        <f>SUMIF(Matrix!G3:G8, E10, Matrix!H3:H8)</f>
-        <v>0.4</v>
+        <f>SUMIF(Matrix!$G$7:$G$8, E10, Matrix!$H$3:$H$7)</f>
+        <v>0</v>
       </c>
       <c r="F11">
-        <f>SUMIF(Matrix!I3:I8, F10, Matrix!J3:J8)</f>
+        <f>SUMIF(Matrix!$I$3:$I$6, F10, Matrix!$J$3:$J$6)</f>
         <v>0.4</v>
       </c>
       <c r="G11">
-        <f>SUMIF(Matrix!K3:K8, G10, Matrix!L3:L8)</f>
+        <f>SUMIF(Matrix!$K$3:$K$6, G10, Matrix!$L$3:$L$6)</f>
         <v>0.4</v>
       </c>
       <c r="H11">
-        <f>SUMIF(Matrix!M3:M9, H10, Matrix!N3:N9)</f>
+        <f>SUMIF(Matrix!$M$3:$M$9, H10, Matrix!$N$3:$N$9)</f>
         <v>0.1</v>
       </c>
       <c r="I11">
-        <f>SUMIF(Matrix!O3:O9, I10, Matrix!P3:P9)</f>
+        <f>SUMIF(Matrix!$O$3:$O$6, I10, Matrix!$P$3:$P$6)</f>
         <v>0.1</v>
       </c>
       <c r="J11">
-        <f>SUMIF(Matrix!Q3:Q9, J10, Matrix!R3:R9)</f>
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J10, Matrix!$R$3:$R$8)</f>
         <v>0.4</v>
       </c>
       <c r="K11">
-        <f>SUMIF(Matrix!S3:S9, K10, Matrix!T3:T9)</f>
+        <f>SUMIF(Matrix!$S$3:$S$6, K10, Matrix!$T$3:$T$6)</f>
         <v>0.4</v>
       </c>
       <c r="L11">
-        <f>SUMIF(Matrix!U3:U9, L10, Matrix!V3:V9)</f>
+        <f>SUMIF(Matrix!$U$3:$U$6, L10, Matrix!$V$3:$V$6)</f>
         <v>0</v>
       </c>
       <c r="M11">
-        <f>SUMIF(Matrix!W3:W9, M10, Matrix!X3:X9)</f>
+        <f>SUMIF(Matrix!$W$3:$W$6, M10, Matrix!$X$3:$X$6)</f>
         <v>0</v>
       </c>
       <c r="N11">
-        <f>SUMIF(Matrix!Y3:Y7, N10, Matrix!Z3:Z7)</f>
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N10, Matrix!$Z$3:$Z$7)</f>
         <v>0.1</v>
       </c>
       <c r="O11">
@@ -1834,7 +1839,7 @@
       </c>
       <c r="P11">
         <f>SUM(B11:G11)</f>
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
@@ -1846,7 +1851,7 @@
       </c>
       <c r="S11" t="b">
         <f>OR(IF(P11&gt;1.9, TRUE), IF(Q11&gt;1.5, TRUE), AND(IF(P11&gt;1.2, TRUE), IF(Q11&gt;1.2, TRUE)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1898,55 +1903,55 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B13">
-        <f>SUMIF(Matrix!A3:A9, B12, Matrix!B3:B9)</f>
+        <f>SUMIF(Matrix!$A$3:$A$6, B12, Matrix!$B$3:$B$6)</f>
         <v>0.2</v>
       </c>
       <c r="C13">
-        <f>SUMIF(Matrix!C3:C8, C12, Matrix!D3:D8)</f>
+        <f>SUMIF(Matrix!$C$3:$C$8, C12, Matrix!$D$3:$D$8)</f>
         <v>0.4</v>
       </c>
       <c r="D13">
-        <f>SUMIF(Matrix!E3:E8, D12, Matrix!F3:F8)</f>
+        <f>SUMIF(Matrix!$E$3:$E$8, D12, Matrix!$F$3:$F$8)</f>
         <v>0.4</v>
       </c>
       <c r="E13">
-        <f>SUMIF(Matrix!G3:G8, E12, Matrix!H3:H8)</f>
-        <v>0.4</v>
+        <f>SUMIF(Matrix!$G$7:$G$8, E12, Matrix!$H$3:$H$7)</f>
+        <v>0</v>
       </c>
       <c r="F13">
-        <f>SUMIF(Matrix!I3:I8, F12, Matrix!J3:J8)</f>
+        <f>SUMIF(Matrix!$I$3:$I$6, F12, Matrix!$J$3:$J$6)</f>
         <v>0.05</v>
       </c>
       <c r="G13">
-        <f>SUMIF(Matrix!K3:K8, G12, Matrix!L3:L8)</f>
+        <f>SUMIF(Matrix!$K$3:$K$6, G12, Matrix!$L$3:$L$6)</f>
         <v>0.4</v>
       </c>
       <c r="H13">
-        <f>SUMIF(Matrix!M3:M9, H12, Matrix!N3:N9)</f>
+        <f>SUMIF(Matrix!$M$3:$M$9, H12, Matrix!$N$3:$N$9)</f>
         <v>0.1</v>
       </c>
       <c r="I13">
-        <f>SUMIF(Matrix!O3:O9, I12, Matrix!P3:P9)</f>
+        <f>SUMIF(Matrix!$O$3:$O$6, I12, Matrix!$P$3:$P$6)</f>
         <v>0.1</v>
       </c>
       <c r="J13">
-        <f>SUMIF(Matrix!Q3:Q9, J12, Matrix!R3:R9)</f>
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J12, Matrix!$R$3:$R$8)</f>
         <v>0.2</v>
       </c>
       <c r="K13">
-        <f>SUMIF(Matrix!S3:S9, K12, Matrix!T3:T9)</f>
+        <f>SUMIF(Matrix!$S$3:$S$6, K12, Matrix!$T$3:$T$6)</f>
         <v>0.2</v>
       </c>
       <c r="L13">
-        <f ca="1">SUMIF(Matrix!U3:V9, L12, Matrix!V3:V9)</f>
+        <f>SUMIF(Matrix!$U$3:$U$6, L12, Matrix!$V$3:$V$6)</f>
         <v>0.3</v>
       </c>
       <c r="M13">
-        <f>SUMIF(Matrix!W3:W9, M12, Matrix!X3:X9)</f>
+        <f>SUMIF(Matrix!$W$3:$W$6, M12, Matrix!$X$3:$X$6)</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>SUMIF(Matrix!Y3:Y7, N12, Matrix!Z3:Z7)</f>
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N12, Matrix!$Z$3:$Z$7)</f>
         <v>0.1</v>
       </c>
       <c r="O13">
@@ -1955,10 +1960,10 @@
       </c>
       <c r="P13">
         <f>SUM(B13:G13)</f>
-        <v>1.85</v>
+        <v>1.4500000000000002</v>
       </c>
       <c r="Q13">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0.90000000000000013</v>
       </c>
       <c r="R13">
@@ -1966,7 +1971,7 @@
         <v>0.4</v>
       </c>
       <c r="S13" t="b">
-        <f ca="1">OR(IF(P13&gt;1.9, TRUE), IF(Q13&gt;1.5, TRUE), AND(IF(P13&gt;1.2, TRUE), IF(Q13&gt;1.2, TRUE)))</f>
+        <f>OR(IF(P13&gt;1.9, TRUE), IF(Q13&gt;1.5, TRUE), AND(IF(P13&gt;1.2, TRUE), IF(Q13&gt;1.2, TRUE)))</f>
         <v>0</v>
       </c>
     </row>
@@ -2019,55 +2024,55 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B15">
-        <f>SUMIF(Matrix!A3:A9, B14, Matrix!B3:B9)</f>
+        <f>SUMIF(Matrix!$A$3:$A$6, B14, Matrix!$B$3:$B$6)</f>
         <v>0.3</v>
       </c>
       <c r="C15">
-        <f>SUMIF(Matrix!C3:C9, C14, Matrix!D3:D9)</f>
+        <f>SUMIF(Matrix!$C$3:$C$8, C14, Matrix!$D$3:$D$8)</f>
         <v>0.05</v>
       </c>
       <c r="D15">
-        <f>SUMIF(Matrix!E3:E9, D14, Matrix!F3:F9)</f>
+        <f>SUMIF(Matrix!$E$3:$E$8, D14, Matrix!$F$3:$F$8)</f>
         <v>0.4</v>
       </c>
       <c r="E15">
-        <f>SUMIF(Matrix!G3:G9, E14, Matrix!H3:H9)</f>
+        <f>SUMIF(Matrix!$G$7:$G$8, E14, Matrix!$H$3:$H$7)</f>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>SUMIF(Matrix!$I$3:$I$6, F14, Matrix!$J$3:$J$6)</f>
+        <v>0.3</v>
+      </c>
+      <c r="G15">
+        <f>SUMIF(Matrix!$K$3:$K$6, G14, Matrix!$L$3:$L$6)</f>
         <v>0.05</v>
       </c>
-      <c r="F15">
-        <f>SUMIF(Matrix!I3:I9, F14, Matrix!J3:J9)</f>
+      <c r="H15">
+        <f>SUMIF(Matrix!$M$3:$M$9, H14, Matrix!$N$3:$N$9)</f>
+        <v>0.2</v>
+      </c>
+      <c r="I15">
+        <f>SUMIF(Matrix!$O$3:$O$6, I14, Matrix!$P$3:$P$6)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J15">
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J14, Matrix!$R$3:$R$8)</f>
+        <v>0.4</v>
+      </c>
+      <c r="K15">
+        <f>SUMIF(Matrix!$S$3:$S$6, K14, Matrix!$T$3:$T$6)</f>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f>SUMIF(Matrix!$U$3:$U$6, L14, Matrix!$V$3:$V$6)</f>
         <v>0.3</v>
       </c>
-      <c r="G15">
-        <f>SUMIF(Matrix!K3:K9, G14, Matrix!L3:L9)</f>
-        <v>0.05</v>
-      </c>
-      <c r="H15">
-        <f>SUMIF(Matrix!M3:M9, H14, Matrix!N3:N9)</f>
+      <c r="M15">
+        <f>SUMIF(Matrix!$W$3:$W$6, M14, Matrix!$X$3:$X$6)</f>
         <v>0.2</v>
       </c>
-      <c r="I15">
-        <f>SUMIF(Matrix!O3:O9, I14, Matrix!P3:P9)</f>
-        <v>0.1</v>
-      </c>
-      <c r="J15">
-        <f>SUMIF(Matrix!Q3:Q9, J14, Matrix!R3:R9)</f>
-        <v>0.4</v>
-      </c>
-      <c r="K15">
-        <f>SUMIF(Matrix!S3:S9, K14, Matrix!T3:T9)</f>
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <f>SUMIF(Matrix!U3:U9, L14, Matrix!V3:V9)</f>
-        <v>0.3</v>
-      </c>
-      <c r="M15">
-        <f>SUMIF(Matrix!W3:W9, M14, Matrix!X3:X9)</f>
-        <v>0.2</v>
-      </c>
       <c r="N15">
-        <f>SUMIF(Matrix!Y3:Y7, N14, Matrix!Z3:Z7)</f>
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N14, Matrix!$Z$3:$Z$7)</f>
         <v>0.4</v>
       </c>
       <c r="O15">
@@ -2076,7 +2081,7 @@
       </c>
       <c r="P15">
         <f>SUM(B15:G15)</f>
-        <v>1.1500000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
@@ -2140,55 +2145,55 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B17">
-        <f>SUMIF(Matrix!A3:A9, B16, Matrix!B3:B9)</f>
+        <f>SUMIF(Matrix!$A$3:$A$6, B16, Matrix!$B$3:$B$6)</f>
         <v>0.4</v>
       </c>
       <c r="C17">
-        <f>SUMIF(Matrix!C3:C8, C16, Matrix!D3:D8)</f>
+        <f>SUMIF(Matrix!$C$3:$C$8, C16, Matrix!$D$3:$D$8)</f>
         <v>0.4</v>
       </c>
       <c r="D17">
-        <f>SUMIF(Matrix!E3:E8, D16, Matrix!F3:F8)</f>
+        <f>SUMIF(Matrix!$E$3:$E$8, D16, Matrix!$F$3:$F$8)</f>
         <v>0.4</v>
       </c>
       <c r="E17">
-        <f>SUMIF(Matrix!G3:G8, E16, Matrix!H3:H8)</f>
-        <v>0.4</v>
+        <f>SUMIF(Matrix!$G$7:$G$8, E16, Matrix!$H$3:$H$7)</f>
+        <v>0</v>
       </c>
       <c r="F17">
-        <f>SUMIF(Matrix!I3:I8, F16, Matrix!J3:J8)</f>
+        <f>SUMIF(Matrix!$I$3:$I$6, F16, Matrix!$J$3:$J$6)</f>
         <v>0.4</v>
       </c>
       <c r="G17">
-        <f>SUMIF(Matrix!K3:K8, G16, Matrix!L3:L8)</f>
+        <f>SUMIF(Matrix!$K$3:$K$6, G16, Matrix!$L$3:$L$6)</f>
         <v>0.4</v>
       </c>
       <c r="H17">
-        <f>SUMIF(Matrix!M3:M9, H16, Matrix!N3:N9)</f>
+        <f>SUMIF(Matrix!$M$3:$M$9, H16, Matrix!$N$3:$N$9)</f>
         <v>0.4</v>
       </c>
       <c r="I17">
-        <f>SUMIF(Matrix!O3:O9, I16, Matrix!P3:P9)</f>
+        <f>SUMIF(Matrix!$O$3:$O$6, I16, Matrix!$P$3:$P$6)</f>
         <v>0.4</v>
       </c>
       <c r="J17">
-        <f>SUMIF(Matrix!Q3:Q9, J16, Matrix!R3:R9)</f>
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J16, Matrix!$R$3:$R$8)</f>
         <v>0.4</v>
       </c>
       <c r="K17">
-        <f>SUMIF(Matrix!S3:S9, K16, Matrix!T3:T9)</f>
+        <f>SUMIF(Matrix!$S$3:$S$6, K16, Matrix!$T$3:$T$6)</f>
         <v>0.4</v>
       </c>
       <c r="L17">
-        <f ca="1">SUMIF(Matrix!U3:V9, L16, Matrix!V3:V9)</f>
+        <f>SUMIF(Matrix!$U$3:$U$6, L16, Matrix!$V$3:$V$6)</f>
         <v>0.4</v>
       </c>
       <c r="M17">
-        <f>SUMIF(Matrix!W3:W9, M16, Matrix!X3:X9)</f>
+        <f>SUMIF(Matrix!$W$3:$W$6, M16, Matrix!$X$3:$X$6)</f>
         <v>0.4</v>
       </c>
       <c r="N17">
-        <f>SUMIF(Matrix!Y3:Y7, N16, Matrix!Z3:Z7)</f>
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N16, Matrix!$Z$3:$Z$7)</f>
         <v>0.4</v>
       </c>
       <c r="O17">
@@ -2197,10 +2202,10 @@
       </c>
       <c r="P17">
         <f>SUM(B17:G17)</f>
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="Q17">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
       <c r="R17">
@@ -2208,7 +2213,7 @@
         <v>0.8</v>
       </c>
       <c r="S17" t="b">
-        <f ca="1">OR(IF(P17&gt;1.9, TRUE), IF(Q17&gt;1.5, TRUE), AND(IF(P17&gt;1.2, TRUE), IF(Q17&gt;1.2, TRUE)))</f>
+        <f>OR(IF(P17&gt;1.9, TRUE), IF(Q17&gt;1.5, TRUE), AND(IF(P17&gt;1.2, TRUE), IF(Q17&gt;1.2, TRUE)))</f>
         <v>1</v>
       </c>
     </row>
@@ -2261,55 +2266,55 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B19">
-        <f>SUMIF(Matrix!A3:A9, B18, Matrix!B3:B9)</f>
+        <f>SUMIF(Matrix!$A$3:$A$6, B18, Matrix!$B$3:$B$6)</f>
         <v>0.3</v>
       </c>
       <c r="C19">
-        <f>SUMIF(Matrix!C3:C9, C18, Matrix!D3:D9)</f>
+        <f>SUMIF(Matrix!$C$3:$C$8, C18, Matrix!$D$3:$D$8)</f>
         <v>0.4</v>
       </c>
       <c r="D19">
-        <f>SUMIF(Matrix!E3:E9, D18, Matrix!F3:F9)</f>
+        <f>SUMIF(Matrix!$E$3:$E$8, D18, Matrix!$F$3:$F$8)</f>
         <v>0.4</v>
       </c>
       <c r="E19">
-        <f>SUMIF(Matrix!G3:G9, E18, Matrix!H3:H9)</f>
+        <f>SUMIF(Matrix!$G$7:$G$8, E18, Matrix!$H$3:$H$7)</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>SUMIF(Matrix!$I$3:$I$6, F18, Matrix!$J$3:$J$6)</f>
+        <v>0.3</v>
+      </c>
+      <c r="G19">
+        <f>SUMIF(Matrix!$K$3:$K$6, G18, Matrix!$L$3:$L$6)</f>
+        <v>0.4</v>
+      </c>
+      <c r="H19">
+        <f>SUMIF(Matrix!$M$3:$M$9, H18, Matrix!$N$3:$N$9)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I19">
+        <f>SUMIF(Matrix!$O$3:$O$6, I18, Matrix!$P$3:$P$6)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J19">
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J18, Matrix!$R$3:$R$8)</f>
+        <v>0.1</v>
+      </c>
+      <c r="K19">
+        <f>SUMIF(Matrix!$S$3:$S$6, K18, Matrix!$T$3:$T$6)</f>
         <v>0.2</v>
       </c>
-      <c r="F19">
-        <f>SUMIF(Matrix!I3:I9, F18, Matrix!J3:J9)</f>
+      <c r="L19">
+        <f>SUMIF(Matrix!$U$3:$U$6, L18, Matrix!$V$3:$V$6)</f>
         <v>0.3</v>
       </c>
-      <c r="G19">
-        <f>SUMIF(Matrix!K3:K9, G18, Matrix!L3:L9)</f>
-        <v>0.4</v>
-      </c>
-      <c r="H19">
-        <f>SUMIF(Matrix!M3:M9, H18, Matrix!N3:N9)</f>
-        <v>0.1</v>
-      </c>
-      <c r="I19">
-        <f>SUMIF(Matrix!O3:O9, I18, Matrix!P3:P9)</f>
-        <v>0.1</v>
-      </c>
-      <c r="J19">
-        <f>SUMIF(Matrix!Q3:Q9, J18, Matrix!R3:R9)</f>
-        <v>0.1</v>
-      </c>
-      <c r="K19">
-        <f>SUMIF(Matrix!S3:S9, K18, Matrix!T3:T9)</f>
-        <v>0.2</v>
-      </c>
-      <c r="L19">
-        <f ca="1">SUMIF(Matrix!U3:V9, L18, Matrix!V3:V9)</f>
-        <v>0.3</v>
-      </c>
       <c r="M19">
-        <f>SUMIF(Matrix!W3:W9, M18, Matrix!X3:X9)</f>
+        <f>SUMIF(Matrix!$W$3:$W$6, M18, Matrix!$X$3:$X$6)</f>
         <v>0</v>
       </c>
       <c r="N19">
-        <f>SUMIF(Matrix!Y3:Y9, N18, Matrix!Z3:Z9)</f>
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N18, Matrix!$Z$3:$Z$7)</f>
         <v>0.1</v>
       </c>
       <c r="O19">
@@ -2318,10 +2323,10 @@
       </c>
       <c r="P19">
         <f>SUM(B19:G19)</f>
-        <v>2</v>
+        <v>1.8000000000000003</v>
       </c>
       <c r="Q19">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="R19">
@@ -2329,7 +2334,128 @@
         <v>0.4</v>
       </c>
       <c r="S19" t="b">
-        <f ca="1">OR(IF(P19&gt;1.9, TRUE), IF(Q19&gt;1.5, TRUE), AND(IF(P19&gt;1.2, TRUE), IF(Q19&gt;1.2, TRUE)))</f>
+        <f>OR(IF(P19&gt;1.9, TRUE), IF(Q19&gt;1.5, TRUE), AND(IF(P19&gt;1.2, TRUE), IF(Q19&gt;1.2, TRUE)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" t="s">
+        <v>46</v>
+      </c>
+      <c r="O20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <f>SUMIF(Matrix!$A$3:$A$6, B20, Matrix!$B$3:$B$6)</f>
+        <v>0.4</v>
+      </c>
+      <c r="C21">
+        <f>SUMIF(Matrix!$C$3:$C$8, C20, Matrix!$D$3:$D$8)</f>
+        <v>0.4</v>
+      </c>
+      <c r="D21">
+        <f>SUMIF(Matrix!$E$3:$E$8, D20, Matrix!$F$3:$F$8)</f>
+        <v>0.4</v>
+      </c>
+      <c r="E21">
+        <f>SUMIF(Matrix!$G$7:$G$8, E20, Matrix!$H$3:$H$7)</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>SUMIF(Matrix!$I$3:$I$6, F20, Matrix!$J$3:$J$6)</f>
+        <v>0.4</v>
+      </c>
+      <c r="G21">
+        <f>SUMIF(Matrix!$K$3:$K$6, G20, Matrix!$L$3:$L$6)</f>
+        <v>0.4</v>
+      </c>
+      <c r="H21">
+        <f>SUMIF(Matrix!$M$3:$M$9, H20, Matrix!$N$3:$N$9)</f>
+        <v>0.4</v>
+      </c>
+      <c r="I21">
+        <f>SUMIF(Matrix!$O$3:$O$6, I20, Matrix!$P$3:$P$6)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J21">
+        <f>SUMIF(Matrix!$Q$3:$Q$8, J20, Matrix!$R$3:$R$8)</f>
+        <v>0.05</v>
+      </c>
+      <c r="K21">
+        <f>SUMIF(Matrix!$S$3:$S$6, K20, Matrix!$T$3:$T$6)</f>
+        <v>0.2</v>
+      </c>
+      <c r="L21">
+        <f>SUMIF(Matrix!$U$3:$U$6, L20, Matrix!$V$3:$V$6)</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>SUMIF(Matrix!$W$3:$W$6, M20, Matrix!$X$3:$X$6)</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f>SUMIF(Matrix!$Y$3:$Y$7, N20, Matrix!$Z$3:$Z$7)</f>
+        <v>0.1</v>
+      </c>
+      <c r="O21">
+        <f>SUMIF(Matrix!AA5:AA11, O20, Matrix!AB5:AB11)</f>
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <f>SUM(B21:G21)</f>
+        <v>2</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" ref="Q21" si="1">SUM(H21:M21)</f>
+        <v>0.75</v>
+      </c>
+      <c r="R21">
+        <f>SUM(N21:O21)</f>
+        <v>0.1</v>
+      </c>
+      <c r="S21" t="b">
+        <f>OR(IF(P21&gt;1.9, TRUE), IF(Q21&gt;1.5, TRUE), AND(IF(P21&gt;1.2, TRUE), IF(Q21&gt;1.2, TRUE)))</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>